<commit_message>
before changing to function
</commit_message>
<xml_diff>
--- a/csdata/B/SI/B4+.xlsx
+++ b/csdata/B/SI/B4+.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Mondeel\Box\CfA\CHANDRA Rates\csdata\B\SI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16719FE8-F4C6-4C28-A660-FB5B6CB83C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -34,25 +43,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -62,55 +73,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -300,309 +307,314 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>351.41</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1.37</v>
       </c>
-      <c r="C2" s="6">
-        <v>0.7549019607843102</v>
-      </c>
-      <c r="D2" s="3">
-        <v>-20.0</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="5">
+        <v>0.75490196078431016</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-20</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>372.69</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>2.72</v>
       </c>
-      <c r="C3" s="6">
-        <v>0.70915032679738</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4">
+      <c r="C3" s="5">
+        <v>0.70915032679737999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>392.52</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>4.71</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.8921568627451002</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>439.96</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>6.61</v>
       </c>
-      <c r="C5" s="6">
-        <v>0.9607843137254903</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4">
+      <c r="C5" s="5">
+        <v>0.96078431372549034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>488.04</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>8.44</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>1.0294117647058805</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="4">
-        <v>556.57</v>
-      </c>
-      <c r="B7" s="5">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>556.57000000000005</v>
+      </c>
+      <c r="B7" s="4">
         <v>10.29</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>1.0980392156862013</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>645.77</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>11.48</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>1.1437908496732003</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>749.28</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>12.63</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>1.1209150326797008</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>878.45</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>12.99</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>1.1666666666666998</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="4">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>1051.46</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>13.5</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>1.1666666666666998</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="4">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>1267.28</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>13.06</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1.1437908496731986</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="4">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>1511.65</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>12.58</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>1.0980392156863008</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="4">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>1760.02</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>11.74</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>1.0065359477124005</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="4">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>2099.39</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>11.05</v>
       </c>
-      <c r="C15" s="6">
-        <v>0.960784313725501</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4">
+      <c r="C15" s="5">
+        <v>0.96078431372550099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>2495.56</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>10.07</v>
       </c>
-      <c r="C16" s="6">
-        <v>0.937908496732101</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4">
+      <c r="C16" s="5">
+        <v>0.93790849673210097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>2935.88</v>
       </c>
-      <c r="B17" s="5">
-        <v>9.2</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.8235294117646603</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4">
+      <c r="B17" s="4">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.82352941176466032</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>3526.29</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>8.44</v>
       </c>
-      <c r="C18" s="6">
-        <v>0.7549019607843093</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4">
-        <v>4162.85</v>
-      </c>
-      <c r="B19" s="5">
+      <c r="C18" s="5">
+        <v>0.75490196078430927</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>4162.8500000000004</v>
+      </c>
+      <c r="B19" s="4">
         <v>7.53</v>
       </c>
-      <c r="C19" s="6">
-        <v>0.6633986928104605</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4">
-        <v>4897.35</v>
-      </c>
-      <c r="B20" s="5">
+      <c r="C19" s="5">
+        <v>0.66339869281046049</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>4897.3500000000004</v>
+      </c>
+      <c r="B20" s="4">
         <v>6.68</v>
       </c>
-      <c r="C20" s="6">
-        <v>0.54901960784313</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4">
+      <c r="C20" s="5">
+        <v>0.54901960784312998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>5682.32</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>6.13</v>
       </c>
-      <c r="C21" s="6">
-        <v>0.50326797385621</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4">
+      <c r="C21" s="5">
+        <v>0.50326797385621003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>6347.07</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>5.54</v>
       </c>
-      <c r="C22" s="6">
-        <v>0.4575163398692901</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
+      <c r="C22" s="5">
+        <v>0.45751633986929008</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>